<commit_message>
Changed Run mode of test case two to no
</commit_message>
<xml_diff>
--- a/EvvntProject/src/data_engine/DataEngine.xlsx
+++ b/EvvntProject/src/data_engine/DataEngine.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="71">
   <si>
     <t>Description</t>
   </si>
@@ -247,7 +247,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -673,9 +673,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="55.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="55.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -717,7 +717,7 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -741,14 +741,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="12" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="31.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="11.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1354,7 +1354,7 @@
       </c>
       <c r="G26" s="7"/>
       <c r="H26" s="1" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:8" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1405,7 +1405,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="23.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="23.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Save The data sheet
</commit_message>
<xml_diff>
--- a/EvvntProject/src/data_engine/DataEngine.xlsx
+++ b/EvvntProject/src/data_engine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19320" windowHeight="5985" tabRatio="535" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16290" windowHeight="5985" tabRatio="535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="Page_Name">Settings!$A$2:$A$8</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <oleSize ref="A1:I16"/>
+  <oleSize ref="A4:G20"/>
 </workbook>
 </file>
 
@@ -528,7 +528,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -575,12 +575,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -611,6 +624,8 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -919,7 +934,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +982,7 @@
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="19" t="s">
         <v>29</v>
       </c>
     </row>
@@ -978,10 +993,10 @@
       <c r="B4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>29</v>
       </c>
     </row>
@@ -995,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M78"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1378,7 +1393,7 @@
       </c>
       <c r="M15" s="16">
         <f ca="1">NOW()</f>
-        <v>42367.824756481481</v>
+        <v>42367.844582754631</v>
       </c>
     </row>
     <row r="16" spans="1:13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
@@ -1448,7 +1463,7 @@
       </c>
       <c r="G18" s="17" t="str">
         <f ca="1">CONCATENATE("TestAccount_",TEXT(M14,"DD/MM/YYYY"),"_",TEXT(M15,"h:mm:ss.00"))</f>
-        <v>TestAccount_29/12/2015_19:47:38.96</v>
+        <v>TestAccount_29/12/2015_20:16:11.95</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>29</v>
@@ -1629,7 +1644,7 @@
       </c>
       <c r="G26" s="2" t="str">
         <f ca="1">CONCATENATE("TestContact_",TEXT(M14,"DD/MM/YYYY"),"_",TEXT(M15,"h:mm:ss.00"))</f>
-        <v>TestContact_29/12/2015_19:47:38.96</v>
+        <v>TestContact_29/12/2015_20:16:11.95</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>29</v>
@@ -1654,7 +1669,7 @@
       </c>
       <c r="G27" s="7" t="str">
         <f ca="1">CONCATENATE(TEXT(M14,"DD/MM/YYYY"),"_",TEXT(M15,"hh"),"_",TEXT(M15,"ss"),"@evvnt.com")</f>
-        <v>29/12/2015_19_39@evvnt.com</v>
+        <v>29/12/2015_20_12@evvnt.com</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>29</v>
@@ -1870,7 +1885,7 @@
       </c>
       <c r="M36" s="15">
         <f ca="1">NOW()</f>
-        <v>42367.824756481481</v>
+        <v>42367.844582754631</v>
       </c>
     </row>
     <row r="37" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1918,7 +1933,7 @@
       </c>
       <c r="G38" s="14" t="str">
         <f ca="1">G18</f>
-        <v>TestAccount_29/12/2015_19:47:38.96</v>
+        <v>TestAccount_29/12/2015_20:16:11.95</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>29</v>
@@ -2079,7 +2094,7 @@
       </c>
       <c r="G45" s="2" t="str">
         <f ca="1">G26</f>
-        <v>TestContact_29/12/2015_19:47:38.96</v>
+        <v>TestContact_29/12/2015_20:16:11.95</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>29</v>

</xml_diff>